<commit_message>
Improved management of unknown country in author address for parsing affiliations
</commit_message>
<xml_diff>
--- a/BiblioParsing/BiblioParsing_RefFiles/Countries.xlsx
+++ b/BiblioParsing/BiblioParsing_RefFiles/Countries.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC265100\PyVenv\BiblioParsing\BiblioParsing\BiblioParsing_RefFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09BAFB1-03D3-4E61-BBA5-D2FCE3A0E395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-27945" yWindow="8325" windowWidth="23775" windowHeight="12915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +19,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$231</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="739">
   <si>
     <t>Country</t>
   </si>
@@ -2236,12 +2242,15 @@
   </si>
   <si>
     <t>(6.82 ,-5,28)</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2393,6 +2402,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2428,6 +2454,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2603,11 +2646,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7222,7 +7265,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>234</v>
+        <v>738</v>
       </c>
       <c r="B231" t="s">
         <v>463</v>
@@ -7241,7 +7284,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F231"/>
+  <autoFilter ref="A1:F231" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>